<commit_message>
Makes new script to combine radiologist input with the machine learning input.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C6D22-F9BD-41AD-A9C8-3A4F11BECA29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD077CB5-740A-432B-9A94-238D7E63BFB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>GaussianNB</t>
+  </si>
+  <si>
+    <t>Accuracy in CV</t>
+  </si>
+  <si>
+    <t>Final accuracy</t>
   </si>
 </sst>
 </file>
@@ -578,27 +584,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3067BB75-CC92-4339-B95A-5CA0863D1050}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -606,7 +616,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -614,7 +624,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -622,7 +632,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -630,7 +640,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -638,7 +648,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -655,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D25560-2EA9-478E-A92D-08017771ED48}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Creates new directories for cherry picked test and training set so that all test images have a radiologist's input. Creates new script for that specific network. Adds new code to implement voting based system for classification.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB6D36C-64EF-4A30-BFE6-1F0C5D42B809}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D19D50F-EA44-4BF2-BF03-C99EACA702D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Results - Exp 1 bilateral" sheetId="5" r:id="rId5"/>
     <sheet name="Redoing experiment" sheetId="6" r:id="rId6"/>
     <sheet name="Better split" sheetId="7" r:id="rId7"/>
+    <sheet name="Cherry Picked Split" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="313">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -764,6 +765,213 @@
   </si>
   <si>
     <t>Classifier output (66%)</t>
+  </si>
+  <si>
+    <t>N10_L.png</t>
+  </si>
+  <si>
+    <t>N10_R.png</t>
+  </si>
+  <si>
+    <t>N11_L.png</t>
+  </si>
+  <si>
+    <t>N11_R.png</t>
+  </si>
+  <si>
+    <t>N12_L.png</t>
+  </si>
+  <si>
+    <t>N13_L.png</t>
+  </si>
+  <si>
+    <t>N13_R.png</t>
+  </si>
+  <si>
+    <t>N14_R.png</t>
+  </si>
+  <si>
+    <t>N16_L.png</t>
+  </si>
+  <si>
+    <t>N16_R.png</t>
+  </si>
+  <si>
+    <t>N17_L.png</t>
+  </si>
+  <si>
+    <t>N17_R.png</t>
+  </si>
+  <si>
+    <t>N18_L.png</t>
+  </si>
+  <si>
+    <t>N18_R.png</t>
+  </si>
+  <si>
+    <t>N19_L.png</t>
+  </si>
+  <si>
+    <t>N19_R.png</t>
+  </si>
+  <si>
+    <t>N1_L.png</t>
+  </si>
+  <si>
+    <t>N1_R.png</t>
+  </si>
+  <si>
+    <t>N23_L.png</t>
+  </si>
+  <si>
+    <t>N23_R.png</t>
+  </si>
+  <si>
+    <t>N2_L.png</t>
+  </si>
+  <si>
+    <t>N2_R.png</t>
+  </si>
+  <si>
+    <t>N3_L.png</t>
+  </si>
+  <si>
+    <t>N3_R.png</t>
+  </si>
+  <si>
+    <t>N4_L.png</t>
+  </si>
+  <si>
+    <t>N5_L.png</t>
+  </si>
+  <si>
+    <t>N5_R.png</t>
+  </si>
+  <si>
+    <t>N6_L.png</t>
+  </si>
+  <si>
+    <t>N7_L.png</t>
+  </si>
+  <si>
+    <t>N7_R.png</t>
+  </si>
+  <si>
+    <t>N8_R.png</t>
+  </si>
+  <si>
+    <t>N9_L.png</t>
+  </si>
+  <si>
+    <t>N9_R.png</t>
+  </si>
+  <si>
+    <t>AD13_L.png</t>
+  </si>
+  <si>
+    <t>AD15_R.png</t>
+  </si>
+  <si>
+    <t>AD16_R.png</t>
+  </si>
+  <si>
+    <t>AD17_L.png</t>
+  </si>
+  <si>
+    <t>AD18_R.png</t>
+  </si>
+  <si>
+    <t>AD19_L.png</t>
+  </si>
+  <si>
+    <t>AD1_L.png</t>
+  </si>
+  <si>
+    <t>AD20_L.png</t>
+  </si>
+  <si>
+    <t>AD22_L.png</t>
+  </si>
+  <si>
+    <t>AD23_L.png</t>
+  </si>
+  <si>
+    <t>AD25_L.png</t>
+  </si>
+  <si>
+    <t>AD27_R.png</t>
+  </si>
+  <si>
+    <t>AD29_R.png</t>
+  </si>
+  <si>
+    <t>AD31_R.png</t>
+  </si>
+  <si>
+    <t>AD33_L.png</t>
+  </si>
+  <si>
+    <t>AD34_R.png</t>
+  </si>
+  <si>
+    <t>AD36_R.png</t>
+  </si>
+  <si>
+    <t>AD3_L.png</t>
+  </si>
+  <si>
+    <t>AD48_R.png</t>
+  </si>
+  <si>
+    <t>AD4_R.png</t>
+  </si>
+  <si>
+    <t>AD15_L.png</t>
+  </si>
+  <si>
+    <t>AD22_R.png</t>
+  </si>
+  <si>
+    <t>AD27_L.png</t>
+  </si>
+  <si>
+    <t>AD29_L.png</t>
+  </si>
+  <si>
+    <t>AD2_R.png</t>
+  </si>
+  <si>
+    <t>AD32_R.png</t>
+  </si>
+  <si>
+    <t>AD35_L.png</t>
+  </si>
+  <si>
+    <t>AD36_L.png</t>
+  </si>
+  <si>
+    <t>AD38_R.png</t>
+  </si>
+  <si>
+    <t>AD3_R.png</t>
+  </si>
+  <si>
+    <t>AD47_L.png</t>
+  </si>
+  <si>
+    <t>AD6_L.png</t>
+  </si>
+  <si>
+    <t>AD7_L.png</t>
+  </si>
+  <si>
+    <t>AD9_L.png</t>
+  </si>
+  <si>
+    <t>Naïve combined output</t>
+  </si>
+  <si>
+    <t>Radiologist output(89%)</t>
   </si>
 </sst>
 </file>
@@ -9561,8 +9769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20D5539-D357-423F-A818-11DD69B4C447}">
   <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E178" sqref="E178:E221"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13627,4 +13835,1550 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.38127225621974398</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.35214388457679602</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.42568027393660302</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.48328903382826499</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.56278733059599895</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.46802736164238101</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.278069908418352</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.126904712172594</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.34085778617495299</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.122874550414414</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.122979515794961</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.45815132048564999</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2.6363433362033301E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.67731031878068804</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1.93534490534277</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1.34905680728227</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1.39494353385168</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.74689730504989105</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1.0038649892967999</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.50606762399137595</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.345858421257078</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.418320598708599</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.26355140558377099</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.489928809122961</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1.61310979439297</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>7.1176302689889101E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.78841923541751202</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1.44206486581063E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.945894960519573</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1.4421543312912301E-3</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.276114718525655</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1.4005968750279299E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.83427774631806295</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1.17545420169445</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.13469359824778501</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.35679965585986001</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1.2527240589111399</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.83770278143471</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.132856754599637</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>3.9194285037401501E-2</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0.90424178668393196</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.434172685427821</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0.29161066787554502</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.47851370586849901</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.41839552317304002</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.46462417448906701</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.102525642531787</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0.57153831968542002</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0.12919397232232599</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0.31799572002711102</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0.59193187084064403</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.306067726225213</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.47309183145650802</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0.21275148197621599</v>
+      </c>
+      <c r="F55">
+        <v>5.5714286000000002E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" t="s">
+        <v>241</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0.47628868300782101</v>
+      </c>
+      <c r="F56">
+        <v>0.34615384599999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>299</v>
+      </c>
+      <c r="B57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0.23080995081538799</v>
+      </c>
+      <c r="F57">
+        <v>0.28533333399999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.65017711595093497</v>
+      </c>
+      <c r="F58">
+        <v>0.20714285799999901</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>301</v>
+      </c>
+      <c r="B59" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>1.08540133661293</v>
+      </c>
+      <c r="F59">
+        <v>0.57571428599999896</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0.133919099500029</v>
+      </c>
+      <c r="F60">
+        <v>1.0666666E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>303</v>
+      </c>
+      <c r="B61" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0.45963143998139599</v>
+      </c>
+      <c r="F61">
+        <v>0.17733333400000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>304</v>
+      </c>
+      <c r="B62" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0.57380544289633895</v>
+      </c>
+      <c r="F62">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>305</v>
+      </c>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1.02323805176822</v>
+      </c>
+      <c r="F63">
+        <v>0.31066666599999898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0.65711276624159198</v>
+      </c>
+      <c r="F64">
+        <v>0.270666666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>307</v>
+      </c>
+      <c r="B65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>9.7585339335031607E-2</v>
+      </c>
+      <c r="F65">
+        <v>5.4285713999999902E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>308</v>
+      </c>
+      <c r="B66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0.33678689329197098</v>
+      </c>
+      <c r="F66">
+        <v>0.21230769199999899</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>309</v>
+      </c>
+      <c r="B67" t="s">
+        <v>241</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0.108295654650418</v>
+      </c>
+      <c r="F67">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0.40783190376601097</v>
+      </c>
+      <c r="F68">
+        <v>0.43166666599999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds new script to create a NN with 1 hidden layer for nonlinear combinations of radiologist and the previous model output and confidence. Adds new ROC curve figures.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D19D50F-EA44-4BF2-BF03-C99EACA702D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F517CF-4461-40AE-87D5-3029FBB32EDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="314">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -972,6 +971,9 @@
   </si>
   <si>
     <t>Radiologist output(89%)</t>
+  </si>
+  <si>
+    <t>NN combined output</t>
   </si>
 </sst>
 </file>
@@ -13839,10 +13841,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13854,9 +13856,10 @@
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -13878,8 +13881,11 @@
       <c r="G1" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -13902,7 +13908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -13925,7 +13931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -13948,7 +13954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -13971,7 +13977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -13994,7 +14000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -14017,7 +14023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -14040,7 +14046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -14063,7 +14069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -14086,7 +14092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -14109,7 +14115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -14132,7 +14138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>255</v>
       </c>
@@ -14155,7 +14161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>256</v>
       </c>
@@ -14178,7 +14184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -14201,7 +14207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>258</v>
       </c>

</xml_diff>

<commit_message>
Adds improveemnts to the breast muscle segmentation script
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F517CF-4461-40AE-87D5-3029FBB32EDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019DF25-8B26-4DE8-8FAD-4EFEBD79212E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="930" windowWidth="24180" windowHeight="11505" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="Redoing experiment" sheetId="6" r:id="rId6"/>
     <sheet name="Better split" sheetId="7" r:id="rId7"/>
     <sheet name="Cherry Picked Split" sheetId="8" r:id="rId8"/>
+    <sheet name="Cherry Picked Cropped" sheetId="9" r:id="rId9"/>
+    <sheet name="Cherry Picked Croppedv5" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="317">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -973,7 +975,16 @@
     <t>Radiologist output(89%)</t>
   </si>
   <si>
-    <t>NN combined output</t>
+    <t>Classifier output (58%)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(83%)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(91%)</t>
+  </si>
+  <si>
+    <t>Classifier output (65%)</t>
   </si>
 </sst>
 </file>
@@ -2461,6 +2472,1272 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05345A79-0C3E-4CB4-94C2-F3400A75A1B0}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E54" sqref="E2:E54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.58397878807507897</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.22412745109266899</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3.51279439461895E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.27180099564495602</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.26747615711157902</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.135093937560993</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.102097985499916</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.459537601370477</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.28111183174036902</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.107666255125386</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.46258461940020701</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.42322147911478802</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.106970489960339</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.50450668261906895</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.28005320741915801</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.64789445228646503</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>5.4057796888002302E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.74730013358171599</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.33414463408869299</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.13615519907318399</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.19803032251682601</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.35992396552103001</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>8.8874312878961595E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1.28580007962729E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.25195750647486398</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.17506402590849601</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0.19883258114799901</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.79129690388674601</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.337629417746872</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.36149375174410198</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.55439828339709296</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.36365360586276402</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.10458301139411</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1.8920125612651901E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>7.4105366657103003E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.27886373991170899</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.13464665399883299</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.21317689635253301</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0.406096641100477</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.91890074019969603</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0.19154549060961301</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.59157603061552899</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>5.6339751832784703E-2</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.17185380400022901</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.29544908738929798</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0.44642350998887997</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>4.6545571380607199E-2</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0.18883748186744101</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>3.03320363517657E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.15744707193678201</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.106422963573294</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3067BB75-CC92-4339-B95A-5CA0863D1050}">
   <dimension ref="A1:C7"/>
@@ -13841,25 +15118,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E68" sqref="E2:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -13881,11 +15158,8 @@
       <c r="G1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -13908,7 +15182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -13931,7 +15205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -13954,7 +15228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -13977,7 +15251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -14000,7 +15274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -14023,7 +15297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -14046,7 +15320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -14069,7 +15343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -14092,7 +15366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -14115,7 +15389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -14138,7 +15412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>255</v>
       </c>
@@ -14161,7 +15435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>256</v>
       </c>
@@ -14184,7 +15458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -14207,7 +15481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>258</v>
       </c>
@@ -15382,6 +16656,1272 @@
       </c>
       <c r="F68">
         <v>0.43166666599999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D98F5B-0C08-4775-B26F-FF5BF735BF93}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.51818056769699705</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.51544979289965598</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.37443502541560503</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.14310428489787699</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.41210641043174001</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>7.5096284941044394E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.65586307369425001</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.41565835139843998</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.26374770683901499</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.42287907623342502</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.234182803209321</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.28232107182368099</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.30633796339499703</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.30190934332684699</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.361855565080626</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.56168499558117002</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.83555648188826204</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.128001194339878</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.47367251197644999</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.41612274926864901</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.31495027004172799</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>3.9177911703948499E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.20836010619826101</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.4037419404116</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.63579022035916999</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>3.3247026193759598E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.67179691255478102</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.51994593489126595</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.22019831497633299</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.231113253288045</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.60165865219660197</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>8.1306414106546501E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.11260709649535799</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>7.7567858732126599E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>3.6743546507149602E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.35698696597920998</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.13096664692370999</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.34368660774169801</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0.137105793622426</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.412405443079286</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>6.0311240407589603E-2</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.32296541569533499</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.27074429016096302</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.377462097703958</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>6.7632881720679997E-4</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>2.6785947742087202E-2</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>5.7030856418948898E-3</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0.38995717483800402</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>8.5036949231722503E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>7.5331752338878094E-2</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.23012641776144499</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates gabor filter SVM
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019DF25-8B26-4DE8-8FAD-4EFEBD79212E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A5B57-F784-42F6-89F3-865A710984FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1935" yWindow="930" windowWidth="24180" windowHeight="11505" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16667,8 +16667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D98F5B-0C08-4775-B26F-FF5BF735BF93}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adds code for gabor dict and gabor feature SVM
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A5B57-F784-42F6-89F3-865A710984FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3866691F-A2D1-4252-A678-636BD59E4197}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="930" windowWidth="24180" windowHeight="11505" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="1485" windowWidth="24180" windowHeight="11505" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="319">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -985,6 +985,12 @@
   </si>
   <si>
     <t>Classifier output (65%)</t>
+  </si>
+  <si>
+    <t>Gabor feature distance classification</t>
+  </si>
+  <si>
+    <t>Gabor features SVM</t>
   </si>
 </sst>
 </file>
@@ -2474,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05345A79-0C3E-4CB4-94C2-F3400A75A1B0}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E54" sqref="E2:E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,9 +2495,11 @@
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2513,8 +2521,14 @@
       <c r="G1" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -2536,8 +2550,14 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -2559,8 +2579,14 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -2582,8 +2608,14 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -2605,8 +2637,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -2628,8 +2666,14 @@
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -2651,8 +2695,14 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -2674,8 +2724,14 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -2697,8 +2753,14 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -2720,8 +2782,14 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -2743,8 +2811,14 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -2766,8 +2840,14 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>255</v>
       </c>
@@ -2789,8 +2869,14 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>256</v>
       </c>
@@ -2812,8 +2898,14 @@
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -2835,8 +2927,14 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>258</v>
       </c>
@@ -2858,8 +2956,14 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -2881,8 +2985,14 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>260</v>
       </c>
@@ -2904,8 +3014,14 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>261</v>
       </c>
@@ -2927,8 +3043,14 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -2950,8 +3072,14 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>263</v>
       </c>
@@ -2973,8 +3101,14 @@
       <c r="G21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>264</v>
       </c>
@@ -2996,8 +3130,14 @@
       <c r="G22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>265</v>
       </c>
@@ -3019,8 +3159,14 @@
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>266</v>
       </c>
@@ -3042,8 +3188,14 @@
       <c r="G24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>267</v>
       </c>
@@ -3065,8 +3217,14 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>268</v>
       </c>
@@ -3088,8 +3246,14 @@
       <c r="G26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>269</v>
       </c>
@@ -3111,8 +3275,14 @@
       <c r="G27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>270</v>
       </c>
@@ -3134,8 +3304,14 @@
       <c r="G28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -3157,8 +3333,14 @@
       <c r="G29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>272</v>
       </c>
@@ -3180,8 +3362,14 @@
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>273</v>
       </c>
@@ -3203,8 +3391,14 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>274</v>
       </c>
@@ -3226,8 +3420,14 @@
       <c r="G32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>275</v>
       </c>
@@ -3249,8 +3449,14 @@
       <c r="G33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>276</v>
       </c>
@@ -3272,8 +3478,14 @@
       <c r="G34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>277</v>
       </c>
@@ -3295,8 +3507,14 @@
       <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>278</v>
       </c>
@@ -3318,8 +3536,14 @@
       <c r="G36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>279</v>
       </c>
@@ -3341,8 +3565,14 @@
       <c r="G37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>280</v>
       </c>
@@ -3364,8 +3594,14 @@
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>281</v>
       </c>
@@ -3387,8 +3623,14 @@
       <c r="G39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>282</v>
       </c>
@@ -3410,8 +3652,14 @@
       <c r="G40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>283</v>
       </c>
@@ -3433,8 +3681,14 @@
       <c r="G41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>284</v>
       </c>
@@ -3456,8 +3710,14 @@
       <c r="G42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>285</v>
       </c>
@@ -3479,8 +3739,14 @@
       <c r="G43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>286</v>
       </c>
@@ -3502,8 +3768,14 @@
       <c r="G44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>287</v>
       </c>
@@ -3525,8 +3797,14 @@
       <c r="G45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>288</v>
       </c>
@@ -3548,8 +3826,14 @@
       <c r="G46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>289</v>
       </c>
@@ -3571,8 +3855,14 @@
       <c r="G47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>290</v>
       </c>
@@ -3594,8 +3884,14 @@
       <c r="G48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>291</v>
       </c>
@@ -3617,8 +3913,14 @@
       <c r="G49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>292</v>
       </c>
@@ -3640,8 +3942,14 @@
       <c r="G50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>293</v>
       </c>
@@ -3663,8 +3971,14 @@
       <c r="G51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>294</v>
       </c>
@@ -3686,8 +4000,14 @@
       <c r="G52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -3709,8 +4029,14 @@
       <c r="G53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>296</v>
       </c>
@@ -3730,6 +4056,12 @@
         <v>0.27</v>
       </c>
       <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
         <v>1</v>
       </c>
     </row>
@@ -16667,8 +16999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D98F5B-0C08-4775-B26F-FF5BF735BF93}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates results after CV shows no improvement.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3866691F-A2D1-4252-A678-636BD59E4197}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A1FEBB-BE83-486E-9292-34EE894E54FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1485" windowWidth="24180" windowHeight="11505" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,8 @@
     <sheet name="Results - Exp 1 bilateral" sheetId="5" r:id="rId5"/>
     <sheet name="Redoing experiment" sheetId="6" r:id="rId6"/>
     <sheet name="Better split" sheetId="7" r:id="rId7"/>
-    <sheet name="Cherry Picked Split" sheetId="8" r:id="rId8"/>
-    <sheet name="Cherry Picked Cropped" sheetId="9" r:id="rId9"/>
+    <sheet name="Cherry Picked Cropped" sheetId="9" r:id="rId8"/>
+    <sheet name="Cherry Picked Split" sheetId="8" r:id="rId9"/>
     <sheet name="Cherry Picked Croppedv5" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="321">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -969,9 +969,6 @@
     <t>AD9_L.png</t>
   </si>
   <si>
-    <t>Naïve combined output</t>
-  </si>
-  <si>
     <t>Radiologist output(89%)</t>
   </si>
   <si>
@@ -981,16 +978,25 @@
     <t>Naïve combined output(83%)</t>
   </si>
   <si>
-    <t>Naïve combined output(91%)</t>
-  </si>
-  <si>
-    <t>Classifier output (65%)</t>
-  </si>
-  <si>
-    <t>Gabor feature distance classification</t>
-  </si>
-  <si>
-    <t>Gabor features SVM</t>
+    <t>Gabor feature distance classification (AUC=0.54)</t>
+  </si>
+  <si>
+    <t>Classifier output (65%, AUC=0.66)</t>
+  </si>
+  <si>
+    <t>Radiologist output(89%, AUC=0.87)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(91%, AUC=0.91)</t>
+  </si>
+  <si>
+    <t>Classifier confidence(r=0.338 with radiologist confidence, p=0.013)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(AUC=0.78)</t>
+  </si>
+  <si>
+    <t>Classifier confidence(r=0.29 p=0.03 with radiologist confidence)</t>
   </si>
 </sst>
 </file>
@@ -2480,26 +2486,26 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05345A79-0C3E-4CB4-94C2-F3400A75A1B0}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2507,28 +2513,25 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>318</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -2553,11 +2556,8 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -2582,11 +2582,8 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -2611,11 +2608,8 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -2640,11 +2634,8 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -2669,11 +2660,8 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -2698,11 +2686,8 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -2727,11 +2712,8 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -2756,11 +2738,8 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -2785,11 +2764,8 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -2814,11 +2790,8 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -2843,11 +2816,8 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>255</v>
       </c>
@@ -2872,11 +2842,8 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>256</v>
       </c>
@@ -2901,11 +2868,8 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -2930,11 +2894,8 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>258</v>
       </c>
@@ -2959,11 +2920,8 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -2988,11 +2946,8 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>260</v>
       </c>
@@ -3017,11 +2972,8 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>261</v>
       </c>
@@ -3046,11 +2998,8 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -3075,11 +3024,8 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>263</v>
       </c>
@@ -3104,11 +3050,8 @@
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>264</v>
       </c>
@@ -3133,11 +3076,8 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>265</v>
       </c>
@@ -3162,11 +3102,8 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>266</v>
       </c>
@@ -3191,11 +3128,8 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>267</v>
       </c>
@@ -3220,11 +3154,8 @@
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>268</v>
       </c>
@@ -3249,11 +3180,8 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>269</v>
       </c>
@@ -3278,11 +3206,8 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>270</v>
       </c>
@@ -3307,11 +3232,8 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -3336,11 +3258,8 @@
       <c r="H29">
         <v>1</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>272</v>
       </c>
@@ -3365,11 +3284,8 @@
       <c r="H30">
         <v>1</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>273</v>
       </c>
@@ -3394,11 +3310,8 @@
       <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>274</v>
       </c>
@@ -3423,11 +3336,8 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>275</v>
       </c>
@@ -3452,11 +3362,8 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>276</v>
       </c>
@@ -3481,11 +3388,8 @@
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>277</v>
       </c>
@@ -3510,11 +3414,8 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>278</v>
       </c>
@@ -3539,11 +3440,8 @@
       <c r="H36">
         <v>0</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>279</v>
       </c>
@@ -3568,11 +3466,8 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>280</v>
       </c>
@@ -3597,11 +3492,8 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>281</v>
       </c>
@@ -3626,11 +3518,8 @@
       <c r="H39">
         <v>1</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>282</v>
       </c>
@@ -3655,11 +3544,8 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>283</v>
       </c>
@@ -3684,11 +3570,8 @@
       <c r="H41">
         <v>1</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>284</v>
       </c>
@@ -3713,11 +3596,8 @@
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>285</v>
       </c>
@@ -3742,11 +3622,8 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>286</v>
       </c>
@@ -3771,11 +3648,8 @@
       <c r="H44">
         <v>1</v>
       </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>287</v>
       </c>
@@ -3800,11 +3674,8 @@
       <c r="H45">
         <v>1</v>
       </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>288</v>
       </c>
@@ -3829,11 +3700,8 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>289</v>
       </c>
@@ -3858,11 +3726,8 @@
       <c r="H47">
         <v>1</v>
       </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>290</v>
       </c>
@@ -3887,11 +3752,8 @@
       <c r="H48">
         <v>0</v>
       </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>291</v>
       </c>
@@ -3916,11 +3778,8 @@
       <c r="H49">
         <v>1</v>
       </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>292</v>
       </c>
@@ -3945,11 +3804,8 @@
       <c r="H50">
         <v>0</v>
       </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>293</v>
       </c>
@@ -3974,11 +3830,8 @@
       <c r="H51">
         <v>0</v>
       </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>294</v>
       </c>
@@ -4003,11 +3856,8 @@
       <c r="H52">
         <v>1</v>
       </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -4032,11 +3882,8 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>296</v>
       </c>
@@ -4060,9 +3907,6 @@
       </c>
       <c r="H54">
         <v>0</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -15449,1553 +15293,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
-  <dimension ref="A1:G68"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E68" sqref="E2:E68"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.38127225621974398</v>
-      </c>
-      <c r="F2">
-        <v>0.462857142</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0.35214388457679602</v>
-      </c>
-      <c r="F3">
-        <v>0.305714285999999</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.42568027393660302</v>
-      </c>
-      <c r="F4">
-        <v>0.54666666600000002</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.48328903382826499</v>
-      </c>
-      <c r="F5">
-        <v>0.40571428599999898</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0.56278733059599895</v>
-      </c>
-      <c r="F6">
-        <v>0.182857142</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>249</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0.46802736164238101</v>
-      </c>
-      <c r="F7">
-        <v>0.29857142799999897</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>250</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0.278069908418352</v>
-      </c>
-      <c r="F8">
-        <v>0.55466666599999903</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0.126904712172594</v>
-      </c>
-      <c r="F9">
-        <v>0.342857142</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0.34085778617495299</v>
-      </c>
-      <c r="F10">
-        <v>4.14285719999999E-2</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>253</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0.122874550414414</v>
-      </c>
-      <c r="F11">
-        <v>0.47538461599999998</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>254</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0.122979515794961</v>
-      </c>
-      <c r="F12">
-        <v>0.54933333399999995</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0.45815132048564999</v>
-      </c>
-      <c r="F13">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>256</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>2.6363433362033301E-2</v>
-      </c>
-      <c r="F14">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>257</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0.67731031878068804</v>
-      </c>
-      <c r="F15">
-        <v>0.347142858</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1.93534490534277</v>
-      </c>
-      <c r="F16">
-        <v>0.61833333399999901</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>259</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>1.34905680728227</v>
-      </c>
-      <c r="F17">
-        <v>0.34153846199999999</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>260</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1.39494353385168</v>
-      </c>
-      <c r="F18">
-        <v>0.37066666599999898</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>261</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0.74689730504989105</v>
-      </c>
-      <c r="F19">
-        <v>0.107999999999999</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>262</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1.0038649892967999</v>
-      </c>
-      <c r="F20">
-        <v>0.62714285800000003</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>263</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0.50606762399137595</v>
-      </c>
-      <c r="F21">
-        <v>0.55333333399999896</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>264</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0.345858421257078</v>
-      </c>
-      <c r="F22">
-        <v>0.37230769199999902</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>265</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0.418320598708599</v>
-      </c>
-      <c r="F23">
-        <v>0.104</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>266</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0.26355140558377099</v>
-      </c>
-      <c r="F24">
-        <v>0.24153846200000001</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>267</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0.489928809122961</v>
-      </c>
-      <c r="F25">
-        <v>0.31733333399999902</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>268</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1.61310979439297</v>
-      </c>
-      <c r="F26">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>269</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>7.1176302689889101E-2</v>
-      </c>
-      <c r="F27">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>270</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0.78841923541751202</v>
-      </c>
-      <c r="F28">
-        <v>0.54533333399999995</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>271</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>1.44206486581063E-2</v>
-      </c>
-      <c r="F29">
-        <v>0.62142857200000001</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>272</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0.945894960519573</v>
-      </c>
-      <c r="F30">
-        <v>0.49333333399999901</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>273</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1.4421543312912301E-3</v>
-      </c>
-      <c r="F31">
-        <v>0.133333334</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>274</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0.276114718525655</v>
-      </c>
-      <c r="F32">
-        <v>0.55733333399999996</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>275</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>1.4005968750279299E-2</v>
-      </c>
-      <c r="F33">
-        <v>0.42307692400000002</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>0.83427774631806295</v>
-      </c>
-      <c r="F34">
-        <v>0.15428571399999899</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>277</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1.17545420169445</v>
-      </c>
-      <c r="F35">
-        <v>0.59285714199999995</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>278</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>0.13469359824778501</v>
-      </c>
-      <c r="F36">
-        <v>0.56666666600000004</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>279</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0.35679965585986001</v>
-      </c>
-      <c r="F37">
-        <v>0.29428571399999998</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>280</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1.2527240589111399</v>
-      </c>
-      <c r="F38">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>281</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>0.83770278143471</v>
-      </c>
-      <c r="F39">
-        <v>0.18266666599999901</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>282</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>0.132856754599637</v>
-      </c>
-      <c r="F40">
-        <v>2.9333333999999898E-2</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>283</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>3.9194285037401501E-2</v>
-      </c>
-      <c r="F41">
-        <v>0.62428571399999999</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>284</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>0.90424178668393196</v>
-      </c>
-      <c r="F42">
-        <v>0.42249999999999999</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>285</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0.434172685427821</v>
-      </c>
-      <c r="F43">
-        <v>0.16666666599999999</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>286</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>0.29161066787554502</v>
-      </c>
-      <c r="F44">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>287</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0.47851370586849901</v>
-      </c>
-      <c r="F45">
-        <v>4.6153839999999403E-3</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>288</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>0.41839552317304002</v>
-      </c>
-      <c r="F46">
-        <v>0.08</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>289</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>0.46462417448906701</v>
-      </c>
-      <c r="F47">
-        <v>0.342857142</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>290</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>0.102525642531787</v>
-      </c>
-      <c r="F48">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>291</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>0.57153831968542002</v>
-      </c>
-      <c r="F49">
-        <v>0.57428571399999995</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>292</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>0.12919397232232599</v>
-      </c>
-      <c r="F50">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>293</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>0.31799572002711102</v>
-      </c>
-      <c r="F51">
-        <v>0.42266666600000002</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>294</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0.59193187084064403</v>
-      </c>
-      <c r="F52">
-        <v>0.30249999999999999</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>295</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0.306067726225213</v>
-      </c>
-      <c r="F53">
-        <v>0.06</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>296</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>0.47309183145650802</v>
-      </c>
-      <c r="F54">
-        <v>0.27</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>297</v>
-      </c>
-      <c r="B55" t="s">
-        <v>241</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55">
-        <v>0.21275148197621599</v>
-      </c>
-      <c r="F55">
-        <v>5.5714286000000002E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>298</v>
-      </c>
-      <c r="B56" t="s">
-        <v>241</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0.47628868300782101</v>
-      </c>
-      <c r="F56">
-        <v>0.34615384599999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>299</v>
-      </c>
-      <c r="B57" t="s">
-        <v>241</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0.23080995081538799</v>
-      </c>
-      <c r="F57">
-        <v>0.28533333399999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>300</v>
-      </c>
-      <c r="B58" t="s">
-        <v>241</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0.65017711595093497</v>
-      </c>
-      <c r="F58">
-        <v>0.20714285799999901</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>301</v>
-      </c>
-      <c r="B59" t="s">
-        <v>241</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>1.08540133661293</v>
-      </c>
-      <c r="F59">
-        <v>0.57571428599999896</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>302</v>
-      </c>
-      <c r="B60" t="s">
-        <v>241</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0.133919099500029</v>
-      </c>
-      <c r="F60">
-        <v>1.0666666E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>303</v>
-      </c>
-      <c r="B61" t="s">
-        <v>241</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>0.45963143998139599</v>
-      </c>
-      <c r="F61">
-        <v>0.17733333400000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>304</v>
-      </c>
-      <c r="B62" t="s">
-        <v>241</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0.57380544289633895</v>
-      </c>
-      <c r="F62">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>305</v>
-      </c>
-      <c r="B63" t="s">
-        <v>241</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>1.02323805176822</v>
-      </c>
-      <c r="F63">
-        <v>0.31066666599999898</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>306</v>
-      </c>
-      <c r="B64" t="s">
-        <v>241</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>0.65711276624159198</v>
-      </c>
-      <c r="F64">
-        <v>0.270666666</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>307</v>
-      </c>
-      <c r="B65" t="s">
-        <v>241</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>9.7585339335031607E-2</v>
-      </c>
-      <c r="F65">
-        <v>5.4285713999999902E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>308</v>
-      </c>
-      <c r="B66" t="s">
-        <v>241</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0.33678689329197098</v>
-      </c>
-      <c r="F66">
-        <v>0.21230769199999899</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>309</v>
-      </c>
-      <c r="B67" t="s">
-        <v>241</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67">
-        <v>0.108295654650418</v>
-      </c>
-      <c r="F67">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>310</v>
-      </c>
-      <c r="B68" t="s">
-        <v>241</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0.40783190376601097</v>
-      </c>
-      <c r="F68">
-        <v>0.43166666599999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D98F5B-0C08-4775-B26F-FF5BF735BF93}">
   <dimension ref="A1:G54"/>
   <sheetViews>
@@ -17022,10 +15319,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -17034,7 +15331,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -18254,6 +16551,1553 @@
       </c>
       <c r="G54">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.38127225621974398</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.35214388457679602</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.42568027393660302</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.48328903382826499</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.56278733059599895</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.46802736164238101</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.278069908418352</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.126904712172594</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.34085778617495299</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.122874550414414</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.122979515794961</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.45815132048564999</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2.6363433362033301E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.67731031878068804</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1.93534490534277</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1.34905680728227</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1.39494353385168</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.74689730504989105</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1.0038649892967999</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.50606762399137595</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.345858421257078</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.418320598708599</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.26355140558377099</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.489928809122961</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1.61310979439297</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>7.1176302689889101E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.78841923541751202</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1.44206486581063E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.945894960519573</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1.4421543312912301E-3</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.276114718525655</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1.4005968750279299E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.83427774631806295</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1.17545420169445</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.13469359824778501</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.35679965585986001</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1.2527240589111399</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.83770278143471</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.132856754599637</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>3.9194285037401501E-2</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0.90424178668393196</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.434172685427821</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0.29161066787554502</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.47851370586849901</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.41839552317304002</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.46462417448906701</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.102525642531787</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0.57153831968542002</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0.12919397232232599</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0.31799572002711102</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0.59193187084064403</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.306067726225213</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.47309183145650802</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0.21275148197621599</v>
+      </c>
+      <c r="F55">
+        <v>5.5714286000000002E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" t="s">
+        <v>241</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0.47628868300782101</v>
+      </c>
+      <c r="F56">
+        <v>0.34615384599999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>299</v>
+      </c>
+      <c r="B57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0.23080995081538799</v>
+      </c>
+      <c r="F57">
+        <v>0.28533333399999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.65017711595093497</v>
+      </c>
+      <c r="F58">
+        <v>0.20714285799999901</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>301</v>
+      </c>
+      <c r="B59" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>1.08540133661293</v>
+      </c>
+      <c r="F59">
+        <v>0.57571428599999896</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0.133919099500029</v>
+      </c>
+      <c r="F60">
+        <v>1.0666666E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>303</v>
+      </c>
+      <c r="B61" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0.45963143998139599</v>
+      </c>
+      <c r="F61">
+        <v>0.17733333400000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>304</v>
+      </c>
+      <c r="B62" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0.57380544289633895</v>
+      </c>
+      <c r="F62">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>305</v>
+      </c>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1.02323805176822</v>
+      </c>
+      <c r="F63">
+        <v>0.31066666599999898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0.65711276624159198</v>
+      </c>
+      <c r="F64">
+        <v>0.270666666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>307</v>
+      </c>
+      <c r="B65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>9.7585339335031607E-2</v>
+      </c>
+      <c r="F65">
+        <v>5.4285713999999902E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>308</v>
+      </c>
+      <c r="B66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0.33678689329197098</v>
+      </c>
+      <c r="F66">
+        <v>0.21230769199999899</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>309</v>
+      </c>
+      <c r="B67" t="s">
+        <v>241</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0.108295654650418</v>
+      </c>
+      <c r="F67">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0.40783190376601097</v>
+      </c>
+      <c r="F68">
+        <v>0.43166666599999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds correlation to excel sheet. Types 2-page paper for Nature Methods first draft
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A1FEBB-BE83-486E-9292-34EE894E54FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E1810-C8F8-4A0B-BA12-628D3CC2BB23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -981,9 +981,6 @@
     <t>Gabor feature distance classification (AUC=0.54)</t>
   </si>
   <si>
-    <t>Classifier output (65%, AUC=0.66)</t>
-  </si>
-  <si>
     <t>Radiologist output(89%, AUC=0.87)</t>
   </si>
   <si>
@@ -997,13 +994,16 @@
   </si>
   <si>
     <t>Classifier confidence(r=0.29 p=0.03 with radiologist confidence)</t>
+  </si>
+  <si>
+    <t>Classifier output (65%, AUC=0.69)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,8 +1019,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,6 +1051,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1057,16 +1093,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1428,6 +1473,636 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Radio</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> confidence vs classifier confidence</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Cherry Picked Croppedv5'!$E$2:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>0.58397878807507897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22412745109266899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.51279439461895E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27180099564495602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26747615711157902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.135093937560993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.102097985499916</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.459537601370477</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28111183174036902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.107666255125386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46258461940020701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42322147911478802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.106970489960339</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.50450668261906895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28005320741915801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64789445228646503</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4057796888002302E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.74730013358171599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.33414463408869299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13615519907318399</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.19803032251682601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.35992396552103001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.8874312878961595E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.28580007962729E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25195750647486398</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.17506402590849601</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.19883258114799901</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79129690388674601</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.337629417746872</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.36149375174410198</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.55439828339709296</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.36365360586276402</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.10458301139411</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8920125612651901E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4105366657103003E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.27886373991170899</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.13464665399883299</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.21317689635253301</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.406096641100477</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.91890074019969603</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.19154549060961301</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.59157603061552899</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.6339751832784703E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.17185380400022901</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.29544908738929798</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.44642350998887997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.6545571380607199E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.18883748186744101</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.03320363517657E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.15744707193678201</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.106422963573294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Cherry Picked Croppedv5'!$F$2:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>0.462857142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.305714285999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54666666600000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40571428599999898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.182857142</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29857142799999897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55466666599999903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.342857142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.14285719999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.47538461599999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.54933333399999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.4000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.347142858</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.61833333399999901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.34153846199999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.37066666599999898</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.107999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.62714285800000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.55333333399999896</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.37230769199999902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.24153846200000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.31733333399999902</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.59599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.34399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.54533333399999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.62142857200000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.49333333399999901</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.133333334</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.55733333399999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.42307692400000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.15428571399999899</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.59285714199999995</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.56666666600000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.29428571399999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.18266666599999901</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.9333333999999898E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.62428571399999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.42249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.16666666599999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.71599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.6153839999999403E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.342857142</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.51200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.57428571399999995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.42266666600000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.30249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BBFD-4BB3-8FB0-4C3635A6603A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="642740936"/>
+        <c:axId val="642742248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="642740936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="642742248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="642742248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="642740936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1468,7 +2143,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2162,6 +3393,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{150B54BE-E17E-47F2-9C29-D483ECE35F91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2486,10 +3758,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05345A79-0C3E-4CB4-94C2-F3400A75A1B0}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,19 +3785,19 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>314</v>
@@ -2635,29 +3907,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.26747615711157902</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0.182857142</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2739,29 +4011,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
         <v>0.459537601370477</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>4.14285719999999E-2</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2817,29 +4089,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
         <v>0.46258461940020701</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2921,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -2946,8 +4218,12 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>PEARSON(E2:E54,F2:F54)</f>
+        <v>6.0299543060194451E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>260</v>
       </c>
@@ -2973,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>261</v>
       </c>
@@ -2999,7 +4275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -3025,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>263</v>
       </c>
@@ -3051,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>264</v>
       </c>
@@ -3077,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>265</v>
       </c>
@@ -3103,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>266</v>
       </c>
@@ -3129,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>267</v>
       </c>
@@ -3155,7 +4431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>268</v>
       </c>
@@ -3181,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>269</v>
       </c>
@@ -3207,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>270</v>
       </c>
@@ -3233,7 +4509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -3259,59 +4535,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
         <v>0.49333333399999901</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
         <v>0.79129690388674601</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>0.133333334</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>274</v>
       </c>
@@ -3363,29 +4639,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
         <v>0.55439828339709296</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>0.15428571399999899</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3441,29 +4717,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
         <v>1.8920125612651901E-2</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="4">
         <v>0.29428571399999998</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3597,29 +4873,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
         <v>0.91890074019969603</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>0.16666666599999999</v>
       </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
+      <c r="G43" s="2">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3649,29 +4925,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
         <v>0.59157603061552899</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>4.6153839999999403E-3</v>
       </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
+      <c r="G45" s="2">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3857,29 +5133,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2">
         <v>0.15744707193678201</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>0.06</v>
       </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53">
+      <c r="G53" s="2">
+        <v>1</v>
+      </c>
+      <c r="H53" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3911,6 +5187,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16562,7 +17839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
@@ -16589,16 +17866,16 @@
         <v>243</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Runs new experiment with different crops
</commit_message>
<xml_diff>
--- a/Solution3/Results/Results.xlsx
+++ b/Solution3/Results/Results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E1810-C8F8-4A0B-BA12-628D3CC2BB23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58006CF7-37B4-4096-98A8-890DD06B7DDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="1665" windowWidth="24180" windowHeight="11505" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial replicaion" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,10 @@
     <sheet name="Better split" sheetId="7" r:id="rId7"/>
     <sheet name="Cherry Picked Cropped" sheetId="9" r:id="rId8"/>
     <sheet name="Cherry Picked Split" sheetId="8" r:id="rId9"/>
-    <sheet name="Cherry Picked Croppedv5" sheetId="10" r:id="rId10"/>
+    <sheet name="Cherry Picked NoCrop" sheetId="12" r:id="rId10"/>
+    <sheet name="Cherry Picked RectCrop" sheetId="11" r:id="rId11"/>
+    <sheet name="Cherry Picked MidCrop" sheetId="13" r:id="rId12"/>
+    <sheet name="Cherry Picked Croppedv5" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="327">
   <si>
     <t>Experiment 1 - Normal vs Cancerous</t>
   </si>
@@ -990,13 +994,31 @@
     <t>Classifier confidence(r=0.338 with radiologist confidence, p=0.013)</t>
   </si>
   <si>
-    <t>Naïve combined output(AUC=0.78)</t>
-  </si>
-  <si>
-    <t>Classifier confidence(r=0.29 p=0.03 with radiologist confidence)</t>
-  </si>
-  <si>
     <t>Classifier output (65%, AUC=0.69)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(75%, AUC=0.84)</t>
+  </si>
+  <si>
+    <t>Classifier output (66%, AUC=0.66)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(75%, AUC=0.78)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(79%, AUC=0.82)</t>
+  </si>
+  <si>
+    <t>Classifier output (69%, AUC=0.72)</t>
+  </si>
+  <si>
+    <t>Classifier output (64%, AUC=0.68)</t>
+  </si>
+  <si>
+    <t>Classifier output (71%, AUC=0.63)</t>
+  </si>
+  <si>
+    <t>Naïve combined output(83%, AUC=0.89)</t>
   </si>
 </sst>
 </file>
@@ -3757,11 +3779,3651 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9D5C02-F553-40D0-AA43-0F8704563EE2}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.19206023831623101</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.445070319625608</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.12246649575134</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.71533265071792695</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.42865579976885898</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.235485559989733</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>4.2410828542746797E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.13468095289530299</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.63155262442668902</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.29975004702223901</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.19619388653660599</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.28160204792527599</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.22908221973130299</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.20845487162864901</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.43094843199107702</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.28592978645574602</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.119114107578879</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.15008566843941701</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.39268281293846702</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.80693399751118999</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.80595213911813202</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.104</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.23824119898034599</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.347507243949851</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.28253714510550398</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.55879251152071296</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.10874213723067599</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0.44601956180747399</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.32602963510847299</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3.2075870741743201E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.16242714225768001</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.66646981013833595</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.67963415948101902</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.37513824919588301</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.52421793249312798</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0.28356503454656601</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.54857852520320105</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.35721033339050301</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.149062818210866</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>7.1795419082496204E-2</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6.3179055840158496E-2</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0.78438523450341302</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.60484931698237598</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.45865572409733701</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.26442817559299597</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.61169278410498595</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0.95829195406289103</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0.95809998769459603</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>8.5071128598106102E-2</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.30531747240135598</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.51728261623643701</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.86416866105012902</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89321AF-DEDB-46C6-A08A-52CA68592553}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.20012358263282001</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.41575528717048199</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.63526897538698801</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.83071681058275904</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.55349120284150599</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.149014057013346</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.312126565881512</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.46923546506660302</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.27485758092322199</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3.73454383091247E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.28827435554743103</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.38029447256084098</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>8.6205696875927898E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.125744102379961</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.21638149424629299</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2.8354133021452701E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.314801874492324</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.13554007750442101</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.115338470295567</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.51778377211465898</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.78838505774882905</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>5.3575359480642799E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.35840662049009098</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.185710938679331</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.21941477739478199</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>6.3622056243856195E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0.506816604145646</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.67873876831692703</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.75887185762515197</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.20317384983300299</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.16105378088326999</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.64755815640395997</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.89906897814152498</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.498655082226232</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.76827987094295802</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>4.9244986729747003E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.29071437292054098</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.44098358836895402</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.97177708962096199</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>3.9133973046436503E-2</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.109254698704753</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>5.8629167916256497E-2</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.197485944248499</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>2.55923110104412E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.65336657519332397</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0.73978678727302005</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0.28033445142865598</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0.33892782097302399</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>4.5832705811284201E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>6.5726194744123098E-2</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.65188091930291903</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4CA6D7-1A6A-4309-A5DF-50D373B750FE}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.58250670819267103</v>
+      </c>
+      <c r="F2">
+        <v>0.462857142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>7.1325417447662201E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.305714285999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.54666666600000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.13457654846911299</v>
+      </c>
+      <c r="F5">
+        <v>0.40571428599999898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.25593795839686601</v>
+      </c>
+      <c r="F6">
+        <v>0.182857142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.126565821418156</v>
+      </c>
+      <c r="F7">
+        <v>0.29857142799999897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.143935565702589</v>
+      </c>
+      <c r="F8">
+        <v>0.55466666599999903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.212998935319274</v>
+      </c>
+      <c r="F9">
+        <v>0.342857142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.49471171667922198</v>
+      </c>
+      <c r="F10">
+        <v>4.14285719999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>9.9741123346675606E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.47538461599999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.185131588916958</v>
+      </c>
+      <c r="F12">
+        <v>0.54933333399999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.249790167385391</v>
+      </c>
+      <c r="F13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>3.8398229514076801E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.119530278401833</v>
+      </c>
+      <c r="F15">
+        <v>0.347142858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.28221228229212503</v>
+      </c>
+      <c r="F16">
+        <v>0.61833333399999901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.20090324871211801</v>
+      </c>
+      <c r="F17">
+        <v>0.34153846199999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.31590280752531003</v>
+      </c>
+      <c r="F18">
+        <v>0.37066666599999898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.53880490654911095</v>
+      </c>
+      <c r="F19">
+        <v>0.107999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>3.4321448756313301E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.62714285800000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>8.93124854045593E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.55333333399999896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.20428631956094201</v>
+      </c>
+      <c r="F22">
+        <v>0.37230769199999902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.31623745918997398</v>
+      </c>
+      <c r="F23">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.20199989863263401</v>
+      </c>
+      <c r="F24">
+        <v>0.24153846200000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.33512531911187998</v>
+      </c>
+      <c r="F25">
+        <v>0.31733333399999902</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>4.8015646133464998E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.32987232077846501</v>
+      </c>
+      <c r="F27">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.59642787353591997</v>
+      </c>
+      <c r="F28">
+        <v>0.54533333399999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>2.9585874583800201E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.62142857200000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>7.0472040570561598E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.49333333399999901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.28120946017092902</v>
+      </c>
+      <c r="F31">
+        <v>0.133333334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>5.3236175936017698E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.55733333399999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.71241437810750696</v>
+      </c>
+      <c r="F33">
+        <v>0.42307692400000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.920708282085827</v>
+      </c>
+      <c r="F34">
+        <v>0.15428571399999899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.81285327977061195</v>
+      </c>
+      <c r="F35">
+        <v>0.59285714199999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0.68775508189967605</v>
+      </c>
+      <c r="F36">
+        <v>0.56666666600000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>2.1431103663960199E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.29428571399999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0.33708357430740199</v>
+      </c>
+      <c r="F38">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.17265378399855799</v>
+      </c>
+      <c r="F39">
+        <v>0.18266666599999901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.40533866406997099</v>
+      </c>
+      <c r="F40">
+        <v>2.9333333999999898E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.69694726081276204</v>
+      </c>
+      <c r="F41">
+        <v>0.62428571399999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>4.62286741723546E-2</v>
+      </c>
+      <c r="F42">
+        <v>0.42249999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.198773986959037</v>
+      </c>
+      <c r="F43">
+        <v>0.16666666599999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0.63164269809616003</v>
+      </c>
+      <c r="F44">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.141443451352362</v>
+      </c>
+      <c r="F45">
+        <v>4.6153839999999403E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0.42425124144273701</v>
+      </c>
+      <c r="F46">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.25603734758408297</v>
+      </c>
+      <c r="F47">
+        <v>0.342857142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0.12166762411804399</v>
+      </c>
+      <c r="F48">
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>0.57428571399999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0.44262474807151703</v>
+      </c>
+      <c r="F50">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>6.6426945386901706E-2</v>
+      </c>
+      <c r="F51">
+        <v>0.42266666600000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0.31017353975843998</v>
+      </c>
+      <c r="F52">
+        <v>0.30249999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.88453746663453203</v>
+      </c>
+      <c r="F53">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.11613527027010399</v>
+      </c>
+      <c r="F54">
+        <v>0.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05345A79-0C3E-4CB4-94C2-F3400A75A1B0}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,7 +7447,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>315</v>
@@ -17839,19 +21501,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285645A5-DA5F-4D75-A674-305233ABEFFB}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17863,19 +21525,19 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>320</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>315</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>319</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>